<commit_message>
LapNV: Complete Rider Favorite List
Signed-off-by: apolong <apolong.lap@gmail.com>
</commit_message>
<xml_diff>
--- a/WIP/Documents/TNET_WebServiceDesign_RIder_v0.3.xlsx
+++ b/WIP/Documents/TNET_WebServiceDesign_RIder_v0.3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="20490" windowHeight="7755" tabRatio="923" firstSheet="24" activeTab="24"/>
+    <workbookView xWindow="0" yWindow="2250" windowWidth="20490" windowHeight="7755" tabRatio="923" firstSheet="14" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Note" sheetId="31" r:id="rId1"/>
@@ -3490,8 +3490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3635,6 +3635,9 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3810,10 +3813,13 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3990,6 +3996,9 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4450,10 +4459,13 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4773,10 +4785,13 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:D6"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4978,6 +4993,9 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5408,10 +5426,13 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="A1:XFD1048576"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5539,10 +5560,13 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5684,7 +5708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
LapNV: Complete Rider Profile
Signed-off-by: apolong <apolong.lap@gmail.com>
</commit_message>
<xml_diff>
--- a/WIP/Documents/TNET_WebServiceDesign_RIder_v0.3.xlsx
+++ b/WIP/Documents/TNET_WebServiceDesign_RIder_v0.3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2250" windowWidth="20490" windowHeight="7755" tabRatio="923" firstSheet="14" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="2700" windowWidth="20490" windowHeight="7755" tabRatio="923" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Note" sheetId="31" r:id="rId1"/>
@@ -3490,7 +3490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4:B6"/>
     </sheetView>
   </sheetViews>
@@ -7550,8 +7550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
LapNV: Update About, Feedback
Signed-off-by: apolong <apolong.lap@gmail.com>
</commit_message>
<xml_diff>
--- a/WIP/Documents/TNET_WebServiceDesign_RIder_v0.3.xlsx
+++ b/WIP/Documents/TNET_WebServiceDesign_RIder_v0.3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2700" windowWidth="20490" windowHeight="7755" tabRatio="923" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="3150" windowWidth="20490" windowHeight="7755" tabRatio="923" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Note" sheetId="31" r:id="rId1"/>
@@ -2369,8 +2369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7550,7 +7550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
LapNV: Completed 90% Rider
Signed-off-by: apolong <apolong.lap@gmail.com>
</commit_message>
<xml_diff>
--- a/WIP/Documents/TNET_WebServiceDesign_RIder_v0.3.xlsx
+++ b/WIP/Documents/TNET_WebServiceDesign_RIder_v0.3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3150" windowWidth="20490" windowHeight="7755" tabRatio="923" firstSheet="3" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="3600" windowWidth="20490" windowHeight="7755" tabRatio="923" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Note" sheetId="31" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="300">
   <si>
     <t>Module Name</t>
   </si>
@@ -200,9 +200,6 @@
     <t>/Logout</t>
   </si>
   <si>
-    <t>/ResetPassword</t>
-  </si>
-  <si>
     <t>POST</t>
   </si>
   <si>
@@ -663,9 +660,6 @@
   </si>
   <si>
     <t>/UpdateAddress</t>
-  </si>
-  <si>
-    <t>/DriverCtr</t>
   </si>
   <si>
     <t>user id</t>
@@ -960,6 +954,9 @@
   </si>
   <si>
     <t>private String uid; private String pw; private String lan; private String cntry; private String cName;</t>
+  </si>
+  <si>
+    <t>/resetPassword</t>
   </si>
 </sst>
 </file>
@@ -2115,22 +2112,22 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -2138,23 +2135,23 @@
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C21" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -2190,7 +2187,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2198,13 +2195,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2224,7 +2221,7 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="31"/>
       <c r="B4" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>5</v>
@@ -2234,7 +2231,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="31"/>
       <c r="B5" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
@@ -2244,7 +2241,7 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
       <c r="B6" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>5</v>
@@ -2259,7 +2256,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="112" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B8" s="62" t="s">
         <v>3</v>
@@ -2274,7 +2271,7 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="113"/>
       <c r="B9" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="15"/>
@@ -2282,7 +2279,7 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="113"/>
       <c r="B10" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="15"/>
@@ -2290,17 +2287,17 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="113"/>
       <c r="B11" s="19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D11" s="15"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="113"/>
       <c r="B12" s="19" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>5</v>
@@ -2310,27 +2307,27 @@
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="113"/>
       <c r="B13" s="19" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D13" s="15"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="113"/>
       <c r="B14" s="19" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D14" s="15"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="113"/>
       <c r="B15" s="19" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>5</v>
@@ -2340,19 +2337,19 @@
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="113"/>
       <c r="B16" s="19" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="114"/>
       <c r="B17" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="18"/>
@@ -2369,7 +2366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2404,7 +2401,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2424,19 +2421,19 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="31"/>
       <c r="B4" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="31"/>
       <c r="B5" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
@@ -2446,7 +2443,7 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
       <c r="B6" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>5</v>
@@ -2456,7 +2453,7 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="31"/>
       <c r="B7" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7" s="34" t="s">
         <v>5</v>
@@ -2466,7 +2463,7 @@
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="31"/>
       <c r="B8" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C8" s="34" t="s">
         <v>5</v>
@@ -2481,7 +2478,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>3</v>
@@ -2496,13 +2493,13 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="31"/>
       <c r="B11" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2557,7 +2554,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>10</v>
@@ -2568,7 +2565,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="129" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>3</v>
@@ -2583,7 +2580,7 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="129"/>
       <c r="B4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>5</v>
@@ -2593,7 +2590,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="129"/>
       <c r="B5" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
@@ -2603,7 +2600,7 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="129"/>
       <c r="B6" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>5</v>
@@ -2613,7 +2610,7 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="129"/>
       <c r="B7" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>5</v>
@@ -2633,13 +2630,13 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="129"/>
       <c r="B9" s="33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C9" s="34" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2651,7 +2648,7 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="129"/>
       <c r="B11" s="33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C11" s="34" t="s">
         <v>5</v>
@@ -2661,73 +2658,73 @@
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="129"/>
       <c r="B12" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" s="15" t="s">
         <v>116</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="129"/>
       <c r="B13" s="71" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="129"/>
       <c r="B14" s="71" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="129"/>
       <c r="B15" s="71" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="129"/>
       <c r="B16" s="71" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="129"/>
       <c r="B17" s="71" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2748,7 +2745,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="112" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>3</v>
@@ -2763,7 +2760,7 @@
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="113"/>
       <c r="B22" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>23</v>
@@ -2813,17 +2810,17 @@
         <v>0</v>
       </c>
       <c r="B1" s="83" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C1" s="84" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="85" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E1" s="86"/>
       <c r="F1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2831,13 +2828,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="88" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="89" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="90" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" s="86"/>
     </row>
@@ -2881,7 +2878,7 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="91"/>
       <c r="B6" s="52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="53" t="s">
         <v>5</v>
@@ -2947,7 +2944,7 @@
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="98"/>
       <c r="B12" s="52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="53" t="s">
         <v>5</v>
@@ -3010,7 +3007,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3018,18 +3015,18 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="112" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>3</v>
@@ -3044,7 +3041,7 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="113"/>
       <c r="B4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>5</v>
@@ -3056,25 +3053,25 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="113"/>
       <c r="B5" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="113"/>
       <c r="B6" s="33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3106,7 +3103,7 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="113"/>
       <c r="B10" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>23</v>
@@ -3161,7 +3158,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3169,13 +3166,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3205,13 +3202,13 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="132"/>
       <c r="B5" s="33" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C5" s="34" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3249,7 +3246,7 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
       <c r="B10" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="15"/>
@@ -3257,7 +3254,7 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
       <c r="B11" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="15"/>
@@ -3265,7 +3262,7 @@
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
       <c r="B12" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="15"/>
@@ -3273,17 +3270,17 @@
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="21"/>
       <c r="B13" s="19" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D13" s="15"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="19" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>5</v>
@@ -3293,7 +3290,7 @@
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="21"/>
       <c r="B15" s="19" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>5</v>
@@ -3303,7 +3300,7 @@
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="21"/>
       <c r="B16" s="19" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>5</v>
@@ -3313,7 +3310,7 @@
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="21"/>
       <c r="B17" s="19" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>5</v>
@@ -3323,7 +3320,7 @@
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="77"/>
       <c r="B18" s="19" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>5</v>
@@ -3333,10 +3330,10 @@
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
       <c r="B19" s="19" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D19" s="15"/>
     </row>
@@ -3513,7 +3510,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3521,13 +3518,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3547,7 +3544,7 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="37"/>
       <c r="B4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>5</v>
@@ -3559,25 +3556,25 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="37"/>
       <c r="B5" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="37"/>
       <c r="B6" s="33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3609,7 +3606,7 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
       <c r="B10" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>5</v>
@@ -3657,13 +3654,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3671,13 +3668,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3703,13 +3700,13 @@
         <v>5</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="37"/>
       <c r="B5" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
@@ -3719,17 +3716,17 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="37"/>
       <c r="B6" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="37"/>
       <c r="B7" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7" s="34" t="s">
         <v>5</v>
@@ -3741,7 +3738,7 @@
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="37"/>
       <c r="B8" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C8" s="34" t="s">
         <v>5</v>
@@ -3753,13 +3750,13 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="37"/>
       <c r="B9" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3779,25 +3776,25 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
       <c r="B11" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
       <c r="B12" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3836,7 +3833,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="83" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" s="84" t="s">
         <v>8</v>
@@ -3845,7 +3842,7 @@
         <v>13</v>
       </c>
       <c r="E1" s="86" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3853,13 +3850,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="88" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="89" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="90" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3879,7 +3876,7 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="91"/>
       <c r="B4" s="95" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" s="53" t="s">
         <v>5</v>
@@ -3895,7 +3892,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="54" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3965,7 +3962,7 @@
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="98"/>
       <c r="B12" s="52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="53" t="s">
         <v>5</v>
@@ -4027,7 +4024,7 @@
         <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -4035,7 +4032,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>10</v>
@@ -4085,7 +4082,7 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="30"/>
       <c r="B6" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C6" s="34" t="s">
         <v>5</v>
@@ -4097,7 +4094,7 @@
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="30"/>
       <c r="B7" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C7" s="34" t="s">
         <v>5</v>
@@ -4109,13 +4106,13 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="30"/>
       <c r="B8" s="38" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="35" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -4141,65 +4138,65 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
       <c r="B11" s="19" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D11" s="15"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
       <c r="B12" s="72" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="21"/>
       <c r="B13" s="58" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="58" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="21"/>
       <c r="B15" s="58" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="21"/>
       <c r="B16" s="58" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>5</v>
@@ -4209,143 +4206,143 @@
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="21"/>
       <c r="B17" s="58" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D17" s="15"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="21"/>
       <c r="B18" s="58" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
       <c r="B19" s="58" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="21"/>
       <c r="B20" s="58" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="21"/>
       <c r="B21" s="58" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="21"/>
       <c r="B22" s="58" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="21"/>
       <c r="B23" s="58" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="21"/>
       <c r="B24" s="58" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="21"/>
       <c r="B25" s="58" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="21"/>
       <c r="B26" s="58" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="21"/>
       <c r="B27" s="58" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="21"/>
       <c r="B28" s="58" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -4438,17 +4435,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="111" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="111" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="111" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -4490,7 +4487,7 @@
         <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -4498,7 +4495,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>10</v>
@@ -4524,7 +4521,7 @@
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="37"/>
       <c r="B4" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="34" t="s">
         <v>5</v>
@@ -4536,7 +4533,7 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="37"/>
       <c r="B5" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="34" t="s">
         <v>5</v>
@@ -4548,13 +4545,13 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="30"/>
       <c r="B6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C6" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D6" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -4589,7 +4586,7 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="77"/>
       <c r="B11" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="15"/>
@@ -4597,7 +4594,7 @@
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="77"/>
       <c r="B12" s="107" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="15"/>
@@ -4605,7 +4602,7 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="77"/>
       <c r="B13" s="108" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="15"/>
@@ -4613,7 +4610,7 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="77"/>
       <c r="B14" s="108" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="15"/>
@@ -4621,7 +4618,7 @@
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="77"/>
       <c r="B15" s="108" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="15"/>
@@ -4629,17 +4626,17 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="77"/>
       <c r="B16" s="108" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="15" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="77"/>
       <c r="B17" s="108" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="15"/>
@@ -4647,7 +4644,7 @@
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="77"/>
       <c r="B18" s="108" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="15"/>
@@ -4813,7 +4810,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4821,13 +4818,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4846,22 +4843,22 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="37" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="37"/>
       <c r="B5" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
@@ -4871,7 +4868,7 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="37"/>
       <c r="B6" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>5</v>
@@ -4918,60 +4915,60 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="74" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="74"/>
       <c r="B13" s="79" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D13" s="15"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="74"/>
       <c r="B14" s="79" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D14" s="15"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="74"/>
       <c r="B15" s="79" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C15" s="34" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="74"/>
       <c r="B16" s="79" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C16" s="34" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -5021,7 +5018,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5029,13 +5026,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5055,7 +5052,7 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="37"/>
       <c r="B4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>5</v>
@@ -5065,7 +5062,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="37"/>
       <c r="B5" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
@@ -5075,7 +5072,7 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="37"/>
       <c r="B6" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>5</v>
@@ -5085,7 +5082,7 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="37"/>
       <c r="B7" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="15"/>
@@ -5093,7 +5090,7 @@
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="37"/>
       <c r="B8" s="19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="15"/>
@@ -5101,7 +5098,7 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="37"/>
       <c r="B9" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="15"/>
@@ -5109,7 +5106,7 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="37"/>
       <c r="B10" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="15"/>
@@ -5117,7 +5114,7 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
       <c r="B11" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="15"/>
@@ -5125,7 +5122,7 @@
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="37"/>
       <c r="B12" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="15"/>
@@ -5133,7 +5130,7 @@
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="37"/>
       <c r="B13" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="15"/>
@@ -5141,7 +5138,7 @@
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="37"/>
       <c r="B14" s="109" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="15"/>
@@ -5149,7 +5146,7 @@
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="37"/>
       <c r="B15" s="109" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="15"/>
@@ -5157,7 +5154,7 @@
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="37"/>
       <c r="B16" s="109" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="15"/>
@@ -5165,7 +5162,7 @@
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="37"/>
       <c r="B17" s="33" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C17" s="34"/>
       <c r="D17" s="35"/>
@@ -5173,7 +5170,7 @@
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="37"/>
       <c r="B18" s="33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C18" s="34"/>
       <c r="D18" s="35"/>
@@ -5181,11 +5178,11 @@
     <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="37"/>
       <c r="B19" s="109" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="110" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -5211,7 +5208,7 @@
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="21"/>
       <c r="B22" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="15"/>
@@ -5219,7 +5216,7 @@
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="21"/>
       <c r="B23" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="15"/>
@@ -5227,13 +5224,13 @@
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="21"/>
       <c r="B24" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -5392,7 +5389,7 @@
       <c r="C50" s="5"/>
       <c r="D50" s="15"/>
       <c r="E50" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -5454,7 +5451,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5462,13 +5459,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5488,7 +5485,7 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="37"/>
       <c r="B4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="15"/>
@@ -5496,7 +5493,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="37"/>
       <c r="B5" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="15"/>
@@ -5504,11 +5501,11 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="37"/>
       <c r="B6" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="15" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -5534,7 +5531,7 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="21"/>
       <c r="B9" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="15"/>
@@ -5542,7 +5539,7 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
       <c r="B10" s="44" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" s="34"/>
       <c r="D10" s="15"/>
@@ -5588,7 +5585,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5596,13 +5593,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5622,7 +5619,7 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="37"/>
       <c r="B4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="15"/>
@@ -5630,7 +5627,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="37"/>
       <c r="B5" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="15"/>
@@ -5638,17 +5635,17 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="37"/>
       <c r="B6" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="15" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="37"/>
       <c r="B7" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>23</v>
@@ -5658,7 +5655,7 @@
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="37"/>
       <c r="B8" s="39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C8" s="34"/>
       <c r="D8" s="13"/>
@@ -5680,7 +5677,7 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="77"/>
       <c r="B10" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="15"/>
@@ -5688,7 +5685,7 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="77"/>
       <c r="B11" s="44" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C11" s="34"/>
       <c r="D11" s="15"/>
@@ -5731,7 +5728,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5739,13 +5736,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5765,7 +5762,7 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="37"/>
       <c r="B4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="15"/>
@@ -5773,7 +5770,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="37"/>
       <c r="B5" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="34"/>
       <c r="D5" s="35"/>
@@ -5781,7 +5778,7 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="37"/>
       <c r="B6" s="39" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C6" s="34"/>
       <c r="D6" s="13"/>
@@ -5809,7 +5806,7 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="21"/>
       <c r="B9" s="33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="15"/>
@@ -5817,7 +5814,7 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
       <c r="B10" s="33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="15"/>
@@ -5825,7 +5822,7 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
       <c r="B11" s="33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="15"/>
@@ -5833,7 +5830,7 @@
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
       <c r="B12" s="33" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="15"/>
@@ -5841,7 +5838,7 @@
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="21"/>
       <c r="B13" s="33" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="15"/>
@@ -5849,7 +5846,7 @@
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="33" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="15"/>
@@ -5857,7 +5854,7 @@
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="21"/>
       <c r="B15" s="33" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="15"/>
@@ -5865,7 +5862,7 @@
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="21"/>
       <c r="B16" s="33" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="15"/>
@@ -5873,7 +5870,7 @@
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="21"/>
       <c r="B17" s="33" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="15"/>
@@ -5881,7 +5878,7 @@
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="21"/>
       <c r="B18" s="33" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="15"/>
@@ -5889,7 +5886,7 @@
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
       <c r="B19" s="33" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="15"/>
@@ -5897,7 +5894,7 @@
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="21"/>
       <c r="B20" s="33" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="15"/>
@@ -5905,7 +5902,7 @@
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="21"/>
       <c r="B21" s="33" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="15"/>
@@ -5913,7 +5910,7 @@
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="21"/>
       <c r="B22" s="33" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="15"/>
@@ -5921,7 +5918,7 @@
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="21"/>
       <c r="B23" s="33" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="15"/>
@@ -5929,7 +5926,7 @@
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="21"/>
       <c r="B24" s="33" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="15"/>
@@ -5937,7 +5934,7 @@
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="21"/>
       <c r="B25" s="33" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="15"/>
@@ -5945,7 +5942,7 @@
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="21"/>
       <c r="B26" s="33" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="15"/>
@@ -5953,7 +5950,7 @@
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="21"/>
       <c r="B27" s="33" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="15"/>
@@ -5961,7 +5958,7 @@
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="21"/>
       <c r="B28" s="33" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="15"/>
@@ -6074,7 +6071,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -6082,13 +6079,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E2" s="40"/>
     </row>
@@ -6109,7 +6106,7 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="37"/>
       <c r="B4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="15"/>
@@ -6117,7 +6114,7 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="37"/>
       <c r="B5" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="15"/>
@@ -6125,7 +6122,7 @@
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="37"/>
       <c r="B6" s="19" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="15"/>
@@ -6133,7 +6130,7 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="37"/>
       <c r="B7" s="19" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="15"/>
@@ -6141,7 +6138,7 @@
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="37"/>
       <c r="B8" s="19" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="15"/>
@@ -6149,7 +6146,7 @@
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="37"/>
       <c r="B9" s="19" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="15"/>
@@ -6157,7 +6154,7 @@
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="37"/>
       <c r="B10" s="19" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="15"/>
@@ -6165,7 +6162,7 @@
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
       <c r="B11" s="38" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="41"/>
@@ -6173,7 +6170,7 @@
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="37"/>
       <c r="B12" s="38" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="41"/>
@@ -6181,7 +6178,7 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="37"/>
       <c r="B13" s="38" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="41"/>
@@ -6189,7 +6186,7 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="37"/>
       <c r="B14" s="33" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C14" s="34"/>
       <c r="D14" s="35"/>
@@ -6211,7 +6208,7 @@
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="21"/>
       <c r="B17" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="15"/>
@@ -6219,7 +6216,7 @@
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="21"/>
       <c r="B18" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="15"/>
@@ -6227,7 +6224,7 @@
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
       <c r="B19" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="15"/>
@@ -6235,7 +6232,7 @@
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="21"/>
       <c r="B20" s="19" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="15"/>
@@ -6243,17 +6240,17 @@
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="80"/>
       <c r="B21" s="19" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="15" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="80"/>
       <c r="B22" s="19" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="15"/>
@@ -6261,7 +6258,7 @@
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="80"/>
       <c r="B23" s="19" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="15"/>
@@ -6269,7 +6266,7 @@
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="80"/>
       <c r="B24" s="19" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="15"/>
@@ -6277,7 +6274,7 @@
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="80"/>
       <c r="B25" s="19" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="15"/>
@@ -6285,7 +6282,7 @@
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="80"/>
       <c r="B26" s="19" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="15"/>
@@ -6293,19 +6290,19 @@
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="80"/>
       <c r="B27" s="19" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="80"/>
       <c r="B28" s="19" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="15"/>
@@ -6313,7 +6310,7 @@
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="80"/>
       <c r="B29" s="19" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="15"/>
@@ -6321,7 +6318,7 @@
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="80"/>
       <c r="B30" s="19" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="15"/>
@@ -6329,7 +6326,7 @@
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="80"/>
       <c r="B31" s="19" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="15"/>
@@ -6337,17 +6334,17 @@
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="80"/>
       <c r="B32" s="19" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D32" s="15"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="80"/>
       <c r="B33" s="19" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>23</v>
@@ -6357,17 +6354,17 @@
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="80"/>
       <c r="B34" s="19" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="15" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="80"/>
       <c r="B35" s="19" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="15"/>
@@ -6375,7 +6372,7 @@
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="80"/>
       <c r="B36" s="19" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="15"/>
@@ -6389,7 +6386,7 @@
     <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="22"/>
       <c r="B38" s="16" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C38" s="17"/>
       <c r="D38" s="18"/>
@@ -6424,7 +6421,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -6432,13 +6429,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E2" s="40"/>
     </row>
@@ -6459,7 +6456,7 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="37"/>
       <c r="B4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="15"/>
@@ -6467,7 +6464,7 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="37"/>
       <c r="B5" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="15"/>
@@ -6475,7 +6472,7 @@
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="37"/>
       <c r="B6" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="15"/>
@@ -6483,7 +6480,7 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="37"/>
       <c r="B7" s="19" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="15"/>
@@ -6491,7 +6488,7 @@
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="37"/>
       <c r="B8" s="19" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="15"/>
@@ -6499,7 +6496,7 @@
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="37"/>
       <c r="B9" s="19" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="15"/>
@@ -6507,7 +6504,7 @@
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="37"/>
       <c r="B10" s="19" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="15"/>
@@ -6515,7 +6512,7 @@
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
       <c r="B11" s="33" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C11" s="34"/>
       <c r="D11" s="35"/>
@@ -6523,7 +6520,7 @@
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="37"/>
       <c r="B12" s="33" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C12" s="34"/>
       <c r="D12" s="35"/>
@@ -6531,7 +6528,7 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="37"/>
       <c r="B13" s="33" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C13" s="34"/>
       <c r="D13" s="35"/>
@@ -6539,7 +6536,7 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="37"/>
       <c r="B14" s="33" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C14" s="34"/>
       <c r="D14" s="35"/>
@@ -6547,7 +6544,7 @@
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="37"/>
       <c r="B15" s="33" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C15" s="34"/>
       <c r="D15" s="35"/>
@@ -6555,7 +6552,7 @@
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="37"/>
       <c r="B16" s="33" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C16" s="34"/>
       <c r="D16" s="35"/>
@@ -6563,7 +6560,7 @@
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="37"/>
       <c r="B17" s="33" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C17" s="34"/>
       <c r="D17" s="35"/>
@@ -6571,7 +6568,7 @@
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="37"/>
       <c r="B18" s="33" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C18" s="34"/>
       <c r="D18" s="35"/>
@@ -6617,7 +6614,7 @@
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="21"/>
       <c r="B24" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="15"/>
@@ -6625,7 +6622,7 @@
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="21"/>
       <c r="B25" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="15"/>
@@ -6799,13 +6796,13 @@
       </c>
       <c r="B2" s="122"/>
       <c r="C2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -6827,7 +6824,7 @@
       <c r="A4" s="117"/>
       <c r="B4" s="118"/>
       <c r="C4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>5</v>
@@ -6840,20 +6837,20 @@
       <c r="A5" s="117"/>
       <c r="B5" s="118"/>
       <c r="C5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="15" t="s">
         <v>79</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="117"/>
       <c r="B6" s="118"/>
       <c r="C6" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>5</v>
@@ -6866,13 +6863,13 @@
       <c r="A7" s="117"/>
       <c r="B7" s="118"/>
       <c r="C7" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="25" t="s">
         <v>179</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -6884,7 +6881,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="112" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B9" s="62" t="s">
         <v>3</v>
@@ -6900,7 +6897,7 @@
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="113"/>
       <c r="B10" s="68" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" s="64"/>
       <c r="D10" s="65" t="s">
@@ -6911,21 +6908,21 @@
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="113"/>
       <c r="B11" s="69" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C11" s="66"/>
       <c r="D11" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E11" s="67"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="113"/>
       <c r="B12" s="123" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C12" s="58" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>5</v>
@@ -6938,7 +6935,7 @@
       <c r="A13" s="113"/>
       <c r="B13" s="124"/>
       <c r="C13" s="58" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>5</v>
@@ -6951,7 +6948,7 @@
       <c r="A14" s="113"/>
       <c r="B14" s="124"/>
       <c r="C14" s="58" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>5</v>
@@ -6977,7 +6974,7 @@
       <c r="A16" s="113"/>
       <c r="B16" s="124"/>
       <c r="C16" s="58" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>5</v>
@@ -6990,7 +6987,7 @@
       <c r="A17" s="113"/>
       <c r="B17" s="124"/>
       <c r="C17" s="58" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>5</v>
@@ -7003,7 +7000,7 @@
       <c r="A18" s="113"/>
       <c r="B18" s="124"/>
       <c r="C18" s="58" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>5</v>
@@ -7016,33 +7013,33 @@
       <c r="A19" s="113"/>
       <c r="B19" s="124"/>
       <c r="C19" s="58" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="113"/>
       <c r="B20" s="124"/>
       <c r="C20" s="58" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="113"/>
       <c r="B21" s="124"/>
       <c r="C21" s="58" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>20</v>
@@ -7055,7 +7052,7 @@
       <c r="A22" s="113"/>
       <c r="B22" s="124"/>
       <c r="C22" s="58" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>20</v>
@@ -7068,7 +7065,7 @@
       <c r="A23" s="113"/>
       <c r="B23" s="124"/>
       <c r="C23" s="58" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>5</v>
@@ -7107,117 +7104,117 @@
       <c r="A26" s="113"/>
       <c r="B26" s="124"/>
       <c r="C26" s="58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="113"/>
       <c r="B27" s="124"/>
       <c r="C27" s="58" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E27" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="113"/>
       <c r="B28" s="124"/>
       <c r="C28" s="58" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D28" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="E28" s="27" t="s">
         <v>182</v>
-      </c>
-      <c r="E28" s="27" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="113"/>
       <c r="B29" s="124"/>
       <c r="C29" s="58" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E29" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="113"/>
       <c r="B30" s="124"/>
       <c r="C30" s="58" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E30" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="113"/>
       <c r="B31" s="124"/>
       <c r="C31" s="58" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E31" s="27" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="113"/>
       <c r="B32" s="124"/>
       <c r="C32" s="58" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="113"/>
       <c r="B33" s="124"/>
       <c r="C33" s="58" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E33" s="27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="113"/>
       <c r="B34" s="124"/>
       <c r="C34" s="58" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E34" s="27" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -7347,13 +7344,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7373,13 +7370,13 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="31"/>
       <c r="B4" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -7397,25 +7394,25 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
       <c r="B6" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="31"/>
       <c r="B7" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -7433,7 +7430,7 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="31"/>
       <c r="B9" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C9" s="34" t="s">
         <v>5</v>
@@ -7445,13 +7442,13 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="31"/>
       <c r="B10" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C10" s="34" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -7474,7 +7471,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="126" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>3</v>
@@ -7499,25 +7496,25 @@
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="127"/>
       <c r="B16" s="33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C16" s="34" t="s">
         <v>43</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="127"/>
       <c r="B17" s="33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" s="34" t="s">
         <v>23</v>
       </c>
       <c r="D17" s="35" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -7550,8 +7547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7581,7 +7578,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>10</v>
@@ -7607,13 +7604,13 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="31"/>
       <c r="B4" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -7631,31 +7628,31 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
       <c r="B6" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="31"/>
       <c r="B7" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="31"/>
       <c r="B8" s="19" t="s">
-        <v>27</v>
+        <v>141</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>5</v>
@@ -7667,7 +7664,7 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="31"/>
       <c r="B9" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C9" s="34" t="s">
         <v>5</v>
@@ -7679,7 +7676,7 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="31"/>
       <c r="B10" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" s="34" t="s">
         <v>5</v>
@@ -7691,13 +7688,13 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="31"/>
       <c r="B11" s="33" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C11" s="34" t="s">
         <v>43</v>
       </c>
       <c r="D11" s="35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -7714,7 +7711,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="126" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>3</v>
@@ -7739,25 +7736,25 @@
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="127"/>
       <c r="B16" s="33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C16" s="34" t="s">
         <v>43</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="127"/>
       <c r="B17" s="33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" s="34" t="s">
         <v>23</v>
       </c>
       <c r="D17" s="35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -7790,8 +7787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7813,7 +7810,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>203</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7821,13 +7818,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7853,13 +7850,13 @@
         <v>5</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="31"/>
       <c r="B5" s="19" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
@@ -7869,13 +7866,13 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
       <c r="B6" s="19" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -7901,23 +7898,23 @@
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="31"/>
       <c r="B9" s="33" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C9" s="34"/>
       <c r="D9" s="81" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="31"/>
       <c r="B10" s="33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -7933,43 +7930,43 @@
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="31"/>
       <c r="B12" s="33" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="31"/>
       <c r="B13" s="33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="31"/>
       <c r="B14" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="31"/>
       <c r="B15" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>5</v>
@@ -8010,7 +8007,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="126" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>3</v>
@@ -8037,13 +8034,13 @@
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="127"/>
       <c r="B24" s="33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24" s="34" t="s">
         <v>23</v>
       </c>
       <c r="D24" s="35" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -8107,7 +8104,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>10</v>
@@ -8139,37 +8136,37 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="31"/>
       <c r="B5" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
       <c r="B6" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>36</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="31"/>
       <c r="B7" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7" s="34" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -8198,7 +8195,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="126" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>3</v>
@@ -8223,17 +8220,17 @@
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="127"/>
       <c r="B14" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="34" t="s">
         <v>103</v>
-      </c>
-      <c r="C14" s="34" t="s">
-        <v>104</v>
       </c>
       <c r="D14" s="35"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="127"/>
       <c r="B15" s="33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C15" s="34" t="s">
         <v>23</v>
@@ -8296,7 +8293,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -8304,7 +8301,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>10</v>
@@ -8313,7 +8310,7 @@
         <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -8386,7 +8383,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="B4:D6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8407,8 +8404,8 @@
       <c r="C1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>9</v>
+      <c r="D1" s="111" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -8416,13 +8413,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>48</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -8457,7 +8454,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="112" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B6" s="62" t="s">
         <v>3</v>
@@ -8472,13 +8469,13 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="113"/>
       <c r="B7" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8492,5 +8489,6 @@
     <mergeCell ref="A6:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
LapNV: Complete Rider Trip
Signed-off-by: apolong <apolong.lap@gmail.com>
</commit_message>
<xml_diff>
--- a/WIP/Documents/TNET_WebServiceDesign_RIder_v0.3.xlsx
+++ b/WIP/Documents/TNET_WebServiceDesign_RIder_v0.3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="20490" windowHeight="7755" tabRatio="923" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="4050" windowWidth="20490" windowHeight="7755" tabRatio="923" firstSheet="8" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Note" sheetId="31" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="301">
   <si>
     <t>Module Name</t>
   </si>
@@ -957,6 +957,9 @@
   </si>
   <si>
     <t>/resetPassword</t>
+  </si>
+  <si>
+    <t>updateDriverStatus</t>
   </si>
 </sst>
 </file>
@@ -4461,8 +4464,8 @@
   </sheetPr>
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4500,8 +4503,8 @@
       <c r="C2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>19</v>
+      <c r="D2" s="111" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -4777,6 +4780,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7547,7 +7551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>